<commit_message>
Check if the types intervention in in evolucare
</commit_message>
<xml_diff>
--- a/service/data/types_interventionV2.xlsx
+++ b/service/data/types_interventionV2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\IFS\nouraures_connector\service\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6620471D-D48E-42E3-A170-CB0104582FBC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D78635C4-D662-4DF7-A954-2CEEE30748BE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="15420" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="types_intervention" sheetId="1" r:id="rId1"/>
@@ -2149,10 +2149,6 @@
     <t>IRM Cérébro-médullaire</t>
   </si>
   <si>
-    <t>IRM Angles ponto-cérébelleux et des CAI (APC et
-CAI), IRM des oreilles</t>
-  </si>
-  <si>
     <t>IRM Faciale/ cervico-faciale</t>
   </si>
   <si>
@@ -2192,10 +2188,6 @@
     <t>IRM Parties molles</t>
   </si>
   <si>
-    <t>IRM Extrémité (bras, avant-bras, cuisse/fémur,
-jambe)</t>
-  </si>
-  <si>
     <t>IRM Rachis cervical</t>
   </si>
   <si>
@@ -2205,10 +2197,6 @@
     <t>IRM Rachis total (médullaire)</t>
   </si>
   <si>
-    <t>IRM Abdominale : hépatique/ pancréatique/ rénale/
-surrénalienne</t>
-  </si>
-  <si>
     <t>IRM Abdomino-pelvienne</t>
   </si>
   <si>
@@ -2393,6 +2381,15 @@
   </si>
   <si>
     <t>MRA06</t>
+  </si>
+  <si>
+    <t>IRM Extrémité (bras, avant-bras, cuisse/fémur,jambe)</t>
+  </si>
+  <si>
+    <t>IRM Angles ponto-cérébelleux et des CAI (APC et CAI), IRM des oreilles</t>
+  </si>
+  <si>
+    <t>IRM Abdominale : hépatique/ pancréatique/ rénale/ surrénalienne</t>
   </si>
 </sst>
 </file>
@@ -3347,22 +3344,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E572"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
-      <selection activeCell="C573" sqref="C573"/>
+    <sheetView tabSelected="1" topLeftCell="A153" workbookViewId="0">
+      <selection activeCell="L168" sqref="L168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="54.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="73.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>606</v>
@@ -3374,7 +3371,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -4110,7 +4107,7 @@
         <v>462</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="D45" s="11">
         <v>5</v>
@@ -4127,7 +4124,7 @@
         <v>463</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="D46" s="11">
         <v>5</v>
@@ -4144,7 +4141,7 @@
         <v>464</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
       <c r="D47" s="11">
         <v>5</v>
@@ -4297,7 +4294,7 @@
         <v>476</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="D56" s="11">
         <v>6</v>
@@ -4689,7 +4686,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="11">
         <v>75</v>
       </c>
@@ -4697,7 +4694,7 @@
         <v>497</v>
       </c>
       <c r="C80" s="12" t="s">
-        <v>704</v>
+        <v>783</v>
       </c>
       <c r="D80" s="11">
         <v>7</v>
@@ -4714,7 +4711,7 @@
         <v>498</v>
       </c>
       <c r="C81" s="12" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D81" s="11">
         <v>7</v>
@@ -4731,7 +4728,7 @@
         <v>499</v>
       </c>
       <c r="C82" s="12" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D82" s="11">
         <v>7</v>
@@ -4748,7 +4745,7 @@
         <v>500</v>
       </c>
       <c r="C83" s="12" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="D83" s="11">
         <v>7</v>
@@ -4762,10 +4759,10 @@
         <v>79</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
       <c r="C84" s="12" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="D84" s="11">
         <v>8</v>
@@ -4796,10 +4793,10 @@
         <v>80</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
       <c r="C86" s="12" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
       <c r="D86" s="11">
         <v>8</v>
@@ -4816,7 +4813,7 @@
         <v>534</v>
       </c>
       <c r="C87" s="12" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="D87" s="11">
         <v>7</v>
@@ -4830,10 +4827,10 @@
         <v>81</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
       <c r="C88" s="12" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="D88" s="11">
         <v>8</v>
@@ -4850,7 +4847,7 @@
         <v>535</v>
       </c>
       <c r="C89" s="12" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="D89" s="11">
         <v>7</v>
@@ -4864,10 +4861,10 @@
         <v>82</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
       <c r="C90" s="12" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="D90" s="11">
         <v>8</v>
@@ -4884,7 +4881,7 @@
         <v>536</v>
       </c>
       <c r="C91" s="12" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="D91" s="11">
         <v>7</v>
@@ -4898,10 +4895,10 @@
         <v>83</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="C92" s="12" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="D92" s="11">
         <v>8</v>
@@ -4918,7 +4915,7 @@
         <v>537</v>
       </c>
       <c r="C93" s="12" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
       <c r="D93" s="11">
         <v>7</v>
@@ -4932,10 +4929,10 @@
         <v>84</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="C94" s="12" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="D94" s="11">
         <v>8</v>
@@ -4952,7 +4949,7 @@
         <v>538</v>
       </c>
       <c r="C95" s="12" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="D95" s="11">
         <v>7</v>
@@ -4966,10 +4963,10 @@
         <v>85</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
       <c r="C96" s="12" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
       <c r="D96" s="11">
         <v>8</v>
@@ -4986,7 +4983,7 @@
         <v>539</v>
       </c>
       <c r="C97" s="12" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="D97" s="11">
         <v>7</v>
@@ -5003,7 +5000,7 @@
         <v>501</v>
       </c>
       <c r="C98" s="12" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D98" s="11">
         <v>7</v>
@@ -5020,7 +5017,7 @@
         <v>502</v>
       </c>
       <c r="C99" s="12" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="D99" s="11">
         <v>7</v>
@@ -5037,7 +5034,7 @@
         <v>503</v>
       </c>
       <c r="C100" s="12" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D100" s="11">
         <v>7</v>
@@ -5051,7 +5048,7 @@
         <v>89</v>
       </c>
       <c r="B101" s="23" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="C101" s="23" t="s">
         <v>282</v>
@@ -5068,7 +5065,7 @@
         <v>90</v>
       </c>
       <c r="B102" s="19" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="C102" s="20" t="s">
         <v>283</v>
@@ -5105,7 +5102,7 @@
         <v>504</v>
       </c>
       <c r="C104" s="12" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D104" s="11">
         <v>7</v>
@@ -5122,7 +5119,7 @@
         <v>505</v>
       </c>
       <c r="C105" s="12" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="D105" s="11">
         <v>7</v>
@@ -5139,7 +5136,7 @@
         <v>506</v>
       </c>
       <c r="C106" s="12" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="D106" s="11">
         <v>7</v>
@@ -5156,7 +5153,7 @@
         <v>507</v>
       </c>
       <c r="C107" s="12" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="D107" s="11">
         <v>7</v>
@@ -5173,7 +5170,7 @@
         <v>508</v>
       </c>
       <c r="C108" s="12" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="D108" s="11">
         <v>7</v>
@@ -5190,7 +5187,7 @@
         <v>509</v>
       </c>
       <c r="C109" s="12" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="D109" s="11">
         <v>7</v>
@@ -5207,7 +5204,7 @@
         <v>510</v>
       </c>
       <c r="C110" s="12" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="D110" s="11">
         <v>7</v>
@@ -5216,7 +5213,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="111" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="11">
         <v>99</v>
       </c>
@@ -5224,7 +5221,7 @@
         <v>511</v>
       </c>
       <c r="C111" s="12" t="s">
-        <v>718</v>
+        <v>782</v>
       </c>
       <c r="D111" s="11">
         <v>7</v>
@@ -5241,7 +5238,7 @@
         <v>512</v>
       </c>
       <c r="C112" s="12" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="D112" s="11">
         <v>7</v>
@@ -5258,7 +5255,7 @@
         <v>513</v>
       </c>
       <c r="C113" s="12" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="D113" s="11">
         <v>7</v>
@@ -5275,7 +5272,7 @@
         <v>514</v>
       </c>
       <c r="C114" s="12" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="D114" s="11">
         <v>7</v>
@@ -5284,7 +5281,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="11">
         <v>103</v>
       </c>
@@ -5292,7 +5289,7 @@
         <v>515</v>
       </c>
       <c r="C115" s="12" t="s">
-        <v>722</v>
+        <v>784</v>
       </c>
       <c r="D115" s="11">
         <v>7</v>
@@ -5360,7 +5357,7 @@
         <v>519</v>
       </c>
       <c r="C119" s="12" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="D119" s="11">
         <v>7</v>
@@ -5377,7 +5374,7 @@
         <v>520</v>
       </c>
       <c r="C120" s="12" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="D120" s="11">
         <v>7</v>
@@ -5394,7 +5391,7 @@
         <v>521</v>
       </c>
       <c r="C121" s="12" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="D121" s="11">
         <v>7</v>
@@ -5445,7 +5442,7 @@
         <v>523</v>
       </c>
       <c r="C124" s="12" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="D124" s="11">
         <v>7</v>
@@ -5462,7 +5459,7 @@
         <v>524</v>
       </c>
       <c r="C125" s="12" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="D125" s="11">
         <v>7</v>
@@ -5479,7 +5476,7 @@
         <v>525</v>
       </c>
       <c r="C126" s="12" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
       <c r="D126" s="11">
         <v>7</v>
@@ -5598,7 +5595,7 @@
         <v>526</v>
       </c>
       <c r="C133" s="12" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
       <c r="D133" s="11">
         <v>7</v>
@@ -5612,7 +5609,7 @@
         <v>470</v>
       </c>
       <c r="B134" s="19" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="C134" s="20" t="s">
         <v>222</v>
@@ -5621,7 +5618,7 @@
         <v>9</v>
       </c>
       <c r="E134" s="18" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -5717,7 +5714,7 @@
         <v>528</v>
       </c>
       <c r="C140" s="12" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
       <c r="D140" s="11">
         <v>7</v>
@@ -5734,7 +5731,7 @@
         <v>529</v>
       </c>
       <c r="C141" s="12" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="D141" s="11">
         <v>7</v>
@@ -5879,7 +5876,7 @@
         <v>530</v>
       </c>
       <c r="C150" s="12" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="D150" s="11">
         <v>7</v>
@@ -5913,7 +5910,7 @@
         <v>532</v>
       </c>
       <c r="C152" s="12" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="D152" s="11">
         <v>7</v>
@@ -5930,7 +5927,7 @@
         <v>489</v>
       </c>
       <c r="C153" s="12" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
       <c r="D153" s="18">
         <v>5</v>
@@ -5947,7 +5944,7 @@
         <v>540</v>
       </c>
       <c r="C154" s="12" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
       <c r="D154" s="11">
         <v>7</v>
@@ -5958,109 +5955,109 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="15" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="B155" s="16" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
       <c r="C155" s="17" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
       <c r="D155" s="15">
         <v>1</v>
       </c>
       <c r="E155" s="15" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="15" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="B156" s="16" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="C156" s="17" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="D156" s="15">
         <v>1</v>
       </c>
       <c r="E156" s="15" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="15" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="B157" s="16" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="C157" s="17" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="D157" s="15">
         <v>1</v>
       </c>
       <c r="E157" s="15" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="15" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="B158" s="16" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
       <c r="C158" s="17" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="D158" s="15">
         <v>1</v>
       </c>
       <c r="E158" s="15" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="15" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="B159" s="16" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
       <c r="C159" s="16" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
       <c r="D159" s="15" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="E159" s="15" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="15" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="B160" s="16" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="C160" s="17" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
       <c r="D160" s="15">
         <v>1</v>
       </c>
       <c r="E160" s="15" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="15" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="B161" s="16" t="s">
         <v>672</v>
@@ -6077,7 +6074,7 @@
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="15" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="B162" s="16" t="s">
         <v>673</v>
@@ -6094,7 +6091,7 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="15" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="B163" s="16" t="s">
         <v>674</v>
@@ -6111,7 +6108,7 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="15" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="B164" s="16" t="s">
         <v>675</v>
@@ -6128,7 +6125,7 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="15" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="B165" s="16" t="s">
         <v>676</v>
@@ -6145,7 +6142,7 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="15" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="B166" s="16" t="s">
         <v>677</v>
@@ -6162,7 +6159,7 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="15" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="B167" s="16" t="s">
         <v>678</v>
@@ -6179,7 +6176,7 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="15" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="B168" s="16" t="s">
         <v>679</v>
@@ -6196,7 +6193,7 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="15" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="B169" s="16" t="s">
         <v>680</v>
@@ -6213,13 +6210,13 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="15" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="B170" s="16" t="s">
         <v>681</v>
       </c>
       <c r="C170" s="17" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="D170" s="15">
         <v>5</v>
@@ -6230,7 +6227,7 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="15" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="B171" s="16" t="s">
         <v>682</v>
@@ -9695,7 +9692,7 @@
         <v>369</v>
       </c>
       <c r="D437" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E437" s="11" t="s">
         <v>605</v>
@@ -9712,7 +9709,7 @@
         <v>369</v>
       </c>
       <c r="D438" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E438" s="11" t="s">
         <v>605</v>
@@ -9729,7 +9726,7 @@
         <v>143</v>
       </c>
       <c r="D439" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E439" s="11" t="s">
         <v>605</v>
@@ -9746,7 +9743,7 @@
         <v>144</v>
       </c>
       <c r="D440" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E440" s="11" t="s">
         <v>605</v>
@@ -9763,7 +9760,7 @@
         <v>145</v>
       </c>
       <c r="D441" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E441" s="11" t="s">
         <v>605</v>
@@ -9780,7 +9777,7 @@
         <v>146</v>
       </c>
       <c r="D442" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E442" s="11" t="s">
         <v>605</v>
@@ -9797,7 +9794,7 @@
         <v>147</v>
       </c>
       <c r="D443" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E443" s="11" t="s">
         <v>605</v>
@@ -9814,7 +9811,7 @@
         <v>370</v>
       </c>
       <c r="D444" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E444" s="11" t="s">
         <v>605</v>
@@ -9831,7 +9828,7 @@
         <v>370</v>
       </c>
       <c r="D445" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E445" s="11" t="s">
         <v>605</v>
@@ -9848,7 +9845,7 @@
         <v>148</v>
       </c>
       <c r="D446" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E446" s="11" t="s">
         <v>605</v>
@@ -9865,7 +9862,7 @@
         <v>371</v>
       </c>
       <c r="D447" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E447" s="11" t="s">
         <v>605</v>
@@ -9882,7 +9879,7 @@
         <v>372</v>
       </c>
       <c r="D448" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E448" s="11" t="s">
         <v>605</v>
@@ -9899,7 +9896,7 @@
         <v>373</v>
       </c>
       <c r="D449" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E449" s="11" t="s">
         <v>605</v>
@@ -9916,7 +9913,7 @@
         <v>374</v>
       </c>
       <c r="D450" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E450" s="11" t="s">
         <v>605</v>
@@ -9933,7 +9930,7 @@
         <v>374</v>
       </c>
       <c r="D451" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E451" s="11" t="s">
         <v>605</v>
@@ -9950,7 +9947,7 @@
         <v>375</v>
       </c>
       <c r="D452" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E452" s="11" t="s">
         <v>605</v>
@@ -9967,7 +9964,7 @@
         <v>375</v>
       </c>
       <c r="D453" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E453" s="11" t="s">
         <v>605</v>
@@ -9984,7 +9981,7 @@
         <v>376</v>
       </c>
       <c r="D454" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E454" s="11" t="s">
         <v>605</v>
@@ -10001,7 +9998,7 @@
         <v>377</v>
       </c>
       <c r="D455" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E455" s="11" t="s">
         <v>605</v>
@@ -10018,7 +10015,7 @@
         <v>378</v>
       </c>
       <c r="D456" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E456" s="11" t="s">
         <v>605</v>
@@ -10035,7 +10032,7 @@
         <v>379</v>
       </c>
       <c r="D457" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E457" s="11" t="s">
         <v>605</v>
@@ -10052,7 +10049,7 @@
         <v>149</v>
       </c>
       <c r="D458" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E458" s="11" t="s">
         <v>605</v>
@@ -10069,7 +10066,7 @@
         <v>150</v>
       </c>
       <c r="D459" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E459" s="11" t="s">
         <v>605</v>
@@ -10086,7 +10083,7 @@
         <v>151</v>
       </c>
       <c r="D460" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E460" s="11" t="s">
         <v>605</v>
@@ -10103,7 +10100,7 @@
         <v>380</v>
       </c>
       <c r="D461" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E461" s="11" t="s">
         <v>605</v>
@@ -10120,7 +10117,7 @@
         <v>381</v>
       </c>
       <c r="D462" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E462" s="11" t="s">
         <v>605</v>
@@ -10135,7 +10132,7 @@
       </c>
       <c r="C463" s="10"/>
       <c r="D463" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E463" s="11" t="s">
         <v>605</v>
@@ -10152,7 +10149,7 @@
         <v>152</v>
       </c>
       <c r="D464" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E464" s="11" t="s">
         <v>605</v>
@@ -10169,7 +10166,7 @@
         <v>162</v>
       </c>
       <c r="D465" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E465" s="11" t="s">
         <v>605</v>
@@ -10186,7 +10183,7 @@
         <v>163</v>
       </c>
       <c r="D466" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E466" s="11" t="s">
         <v>605</v>
@@ -10203,7 +10200,7 @@
         <v>164</v>
       </c>
       <c r="D467" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E467" s="11" t="s">
         <v>605</v>
@@ -10220,7 +10217,7 @@
         <v>165</v>
       </c>
       <c r="D468" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E468" s="11" t="s">
         <v>605</v>
@@ -10237,7 +10234,7 @@
         <v>166</v>
       </c>
       <c r="D469" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E469" s="11" t="s">
         <v>605</v>
@@ -10254,7 +10251,7 @@
         <v>167</v>
       </c>
       <c r="D470" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E470" s="11" t="s">
         <v>605</v>
@@ -10271,7 +10268,7 @@
         <v>168</v>
       </c>
       <c r="D471" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E471" s="11" t="s">
         <v>605</v>
@@ -10288,7 +10285,7 @@
         <v>386</v>
       </c>
       <c r="D472" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E472" s="11" t="s">
         <v>605</v>
@@ -10305,7 +10302,7 @@
         <v>387</v>
       </c>
       <c r="D473" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E473" s="11" t="s">
         <v>605</v>
@@ -10322,7 +10319,7 @@
         <v>195</v>
       </c>
       <c r="D474" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E474" s="11" t="s">
         <v>605</v>
@@ -10339,7 +10336,7 @@
         <v>204</v>
       </c>
       <c r="D475" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E475" s="11" t="s">
         <v>605</v>
@@ -10356,7 +10353,7 @@
         <v>206</v>
       </c>
       <c r="D476" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E476" s="11" t="s">
         <v>605</v>
@@ -10373,7 +10370,7 @@
         <v>401</v>
       </c>
       <c r="D477" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E477" s="11" t="s">
         <v>605</v>
@@ -10390,7 +10387,7 @@
         <v>407</v>
       </c>
       <c r="D478" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E478" s="11" t="s">
         <v>605</v>
@@ -10407,7 +10404,7 @@
         <v>218</v>
       </c>
       <c r="D479" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E479" s="11" t="s">
         <v>605</v>
@@ -10424,7 +10421,7 @@
         <v>234</v>
       </c>
       <c r="D480" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E480" s="11" t="s">
         <v>605</v>
@@ -10441,7 +10438,7 @@
         <v>246</v>
       </c>
       <c r="D481" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E481" s="11" t="s">
         <v>605</v>
@@ -10458,7 +10455,7 @@
         <v>247</v>
       </c>
       <c r="D482" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E482" s="11" t="s">
         <v>605</v>
@@ -10475,7 +10472,7 @@
         <v>248</v>
       </c>
       <c r="D483" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E483" s="11" t="s">
         <v>605</v>
@@ -10492,7 +10489,7 @@
         <v>261</v>
       </c>
       <c r="D484" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E484" s="11" t="s">
         <v>605</v>
@@ -10509,7 +10506,7 @@
         <v>262</v>
       </c>
       <c r="D485" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E485" s="11" t="s">
         <v>605</v>
@@ -10526,7 +10523,7 @@
         <v>275</v>
       </c>
       <c r="D486" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E486" s="11" t="s">
         <v>605</v>
@@ -10543,7 +10540,7 @@
         <v>280</v>
       </c>
       <c r="D487" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E487" s="11" t="s">
         <v>605</v>
@@ -10560,7 +10557,7 @@
         <v>281</v>
       </c>
       <c r="D488" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E488" s="11" t="s">
         <v>605</v>
@@ -10577,7 +10574,7 @@
         <v>416</v>
       </c>
       <c r="D489" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E489" s="11" t="s">
         <v>605</v>
@@ -11482,7 +11479,7 @@
     </row>
     <row r="559" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A559" s="15" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="B559" s="16" t="s">
         <v>683</v>
@@ -11529,7 +11526,7 @@
     </row>
     <row r="562" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A562" s="15" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="B562" s="16" t="s">
         <v>684</v>
@@ -11618,12 +11615,12 @@
     </row>
     <row r="571" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C571" s="13" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
     </row>
     <row r="572" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C572" s="14" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
     </row>
   </sheetData>

</xml_diff>